<commit_message>
updating prsentation - RL
</commit_message>
<xml_diff>
--- a/data/app_trader_application_metrics.xlsx
+++ b/data/app_trader_application_metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\nss-data-analytics\projects\app-trader-thesaurus-rex\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FF081347-EB7B-4C5B-90B9-2B6302B2B858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2476270F-D5DD-4304-AAEC-FB4A5D74C3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20565" yWindow="-1440" windowWidth="19185" windowHeight="10200"/>
+    <workbookView xWindow="195" yWindow="3135" windowWidth="43185" windowHeight="21990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="playstore_rating_metrics" sheetId="2" r:id="rId1"/>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1266,6 +1266,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1390121103"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1386,11 +1387,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Google</a:t>
+              <a:t>Apple Appstore </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Playstore Genre</a:t>
+              <a:t>Genre</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2034,7 +2035,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-1CA2-4285-AAA9-FD9D727F0C36}"/>
                   </c:ext>
@@ -2527,11 +2528,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Google</a:t>
+              <a:t>Apple</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Playstore Genre</a:t>
+              <a:t> Appstore Genre</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3175,7 +3176,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-0F5F-423B-8F9F-2D7542A1069A}"/>
                   </c:ext>
@@ -3664,11 +3665,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Google</a:t>
+              <a:t>Apple Appstore </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Playstore Genre</a:t>
+              <a:t>Genre</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -4311,7 +4312,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-B2B3-463F-A925-9E18C19D591C}"/>
                   </c:ext>
@@ -4516,7 +4517,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-B2B3-463F-A925-9E18C19D591C}"/>
                   </c:ext>
@@ -4744,7 +4745,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Google Playstore</a:t>
+              <a:t>Playstore AVG Ratings</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5045,7 +5046,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-7E7B-415C-8CF0-58787D4616FD}"/>
                   </c:ext>
@@ -5136,7 +5137,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-7E7B-415C-8CF0-58787D4616FD}"/>
                   </c:ext>
@@ -5261,37 +5262,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5672,7 +5642,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-4FF8-434C-8089-733BB22464DE}"/>
                   </c:ext>
@@ -5763,7 +5733,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-4FF8-434C-8089-733BB22464DE}"/>
                   </c:ext>
@@ -6299,7 +6269,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-C831-4B3C-BAFD-D7C3E12EE4D6}"/>
                   </c:ext>
@@ -6390,7 +6360,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-C831-4B3C-BAFD-D7C3E12EE4D6}"/>
                   </c:ext>
@@ -7143,6 +7113,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1390148975"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -7235,10 +7206,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="106"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="6"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -7249,13 +7220,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -7281,13 +7258,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -7319,13 +7302,45 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="86000"/>
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="86000"/>
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:shade val="86000"/>
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -7411,13 +7426,45 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
+                  <a:gradFill rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:schemeClr val="accent4">
+                          <a:shade val="58000"/>
+                          <a:satMod val="103000"/>
+                          <a:lumMod val="102000"/>
+                          <a:tint val="94000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="50000">
+                        <a:schemeClr val="accent4">
+                          <a:shade val="58000"/>
+                          <a:satMod val="110000"/>
+                          <a:lumMod val="100000"/>
+                          <a:shade val="100000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:schemeClr val="accent4">
+                          <a:shade val="58000"/>
+                          <a:lumMod val="99000"/>
+                          <a:satMod val="120000"/>
+                          <a:shade val="78000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="0"/>
+                  </a:gradFill>
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst/>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
                 <c:cat>
@@ -7502,13 +7549,45 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent3"/>
-                  </a:solidFill>
+                  <a:gradFill rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:schemeClr val="accent4">
+                          <a:tint val="86000"/>
+                          <a:satMod val="103000"/>
+                          <a:lumMod val="102000"/>
+                          <a:tint val="94000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="50000">
+                        <a:schemeClr val="accent4">
+                          <a:tint val="86000"/>
+                          <a:satMod val="110000"/>
+                          <a:lumMod val="100000"/>
+                          <a:shade val="100000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:schemeClr val="accent4">
+                          <a:tint val="86000"/>
+                          <a:lumMod val="99000"/>
+                          <a:satMod val="120000"/>
+                          <a:shade val="78000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="0"/>
+                  </a:gradFill>
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst/>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
                 <c:cat>
@@ -7564,7 +7643,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-DA62-498D-B042-E9EFF3F5A670}"/>
                   </c:ext>
@@ -7613,13 +7692,21 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="28575" cap="rnd">
+                  <a:ln w="34925" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent4"/>
+                      <a:schemeClr val="accent4">
+                        <a:tint val="58000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
-                  <a:effectLst/>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
                 </c:spPr>
                 <c:marker>
                   <c:symbol val="none"/>
@@ -7701,11 +7788,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -7719,9 +7806,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -7750,9 +7836,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -7778,9 +7864,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -7853,9 +7938,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -7872,17 +7956,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -8240,7 +8335,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-ECD8-407A-90C1-97DAC48726F2}"/>
                   </c:ext>
@@ -8915,7 +9010,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-C538-4C12-805B-9B4F16D55D18}"/>
                   </c:ext>
@@ -9006,7 +9101,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-C538-4C12-805B-9B4F16D55D18}"/>
                   </c:ext>
@@ -9233,12 +9328,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Google</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Playstore Genre</a:t>
+              <a:t>Apple Appstore Genre</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -10213,6 +10304,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1400623087"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -10619,42 +10711,8 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -14803,35 +14861,33 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -14839,26 +14895,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -14867,9 +14931,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -14888,14 +14951,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -14904,20 +14959,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -14926,13 +14981,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -14944,10 +14999,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -14956,16 +15011,17 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -14983,21 +15039,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -15007,130 +15060,129 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="75000"/>
             <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -15143,14 +15195,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -15159,14 +15210,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -15174,7 +15224,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -15187,11 +15237,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -15199,14 +15259,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -15218,12 +15278,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -15239,7 +15306,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -15248,9 +15314,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -15260,19 +15325,29 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -15281,9 +15356,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -15295,12 +15369,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -17278,8 +17346,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="Everyone"/>
@@ -17290,67 +17358,67 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="content_rating"/>
-    <tableColumn id="2" name="count"/>
-    <tableColumn id="3" name="avg_rating"/>
-    <tableColumn id="4" name="high_rated_total"/>
-    <tableColumn id="5" name="pct_high_rated" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="content_rating"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="count"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="avg_rating"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="high_rated_total"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="pct_high_rated" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="content_rating"/>
-    <tableColumn id="2" name="count"/>
-    <tableColumn id="3" name="avg_rating"/>
-    <tableColumn id="4" name="high_rated_total"/>
-    <tableColumn id="5" name="pct_highly_rated" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="content_rating"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="count"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="avg_rating"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="high_rated_total"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="pct_highly_rated" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:E24" totalsRowShown="0">
-  <autoFilter ref="A1:E24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:E24" totalsRowShown="0">
+  <autoFilter ref="A1:E24" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="primary_genre"/>
-    <tableColumn id="2" name="count"/>
-    <tableColumn id="3" name="avg_rating"/>
-    <tableColumn id="4" name="high_rated_total"/>
-    <tableColumn id="5" name="pct_high_rated" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="primary_genre"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="count"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="avg_rating"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="high_rated_total"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="pct_high_rated" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:F2" totalsRowShown="0" dataCellStyle="Percent">
-  <autoFilter ref="A1:F2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table15" displayName="Table15" ref="A1:F2" totalsRowShown="0" dataCellStyle="Percent">
+  <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="everyone_pct" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="everyone10_pct" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="teen_pct" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="mature_pct" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="adult_pct" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="unrated_pct" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="everyone_pct" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="everyone10_pct" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="teen_pct" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="mature_pct" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="adult_pct" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="unrated_pct" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A1:D2" totalsRowShown="0" dataCellStyle="Percent">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table16" displayName="Table16" ref="A1:D2" totalsRowShown="0" dataCellStyle="Percent">
+  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="everyone_pct" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="everyone9_pct" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="teen_pct" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="mature_pct" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="everyone_pct" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="everyone9_pct" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="teen_pct" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="mature_pct" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17652,10 +17720,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -17779,11 +17847,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17888,11 +17956,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18321,7 +18389,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18387,7 +18455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>